<commit_message>
edited excel assets sheet
</commit_message>
<xml_diff>
--- a/Bryan spul/assetlist borrelbrouwer v2.xlsx
+++ b/Bryan spul/assetlist borrelbrouwer v2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\P10EduGame\Bryan spul\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -93,9 +98,6 @@
     <t>particles</t>
   </si>
   <si>
-    <t>vuur particles</t>
-  </si>
-  <si>
     <t>elektriciteit particle</t>
   </si>
   <si>
@@ -163,12 +165,15 @@
   </si>
   <si>
     <t>main menu</t>
+  </si>
+  <si>
+    <t>vuur particle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -373,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -643,18 +648,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +804,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="10" t="s">
@@ -809,7 +814,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="9" t="s">
@@ -819,7 +824,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="10" t="s">
@@ -853,7 +858,7 @@
     </row>
     <row r="21" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="18"/>
@@ -919,77 +924,77 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="25"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="23"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="23"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="23"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="23"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" s="26"/>
     </row>
     <row r="35" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="18"/>
@@ -997,7 +1002,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
@@ -1005,7 +1010,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
@@ -1013,7 +1018,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
@@ -1021,7 +1026,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
@@ -1029,7 +1034,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
@@ -1037,7 +1042,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
@@ -1045,7 +1050,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
@@ -1053,7 +1058,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
@@ -1061,7 +1066,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
@@ -1069,7 +1074,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="7"/>

</xml_diff>

<commit_message>
Edited assets list, Check Trello for the google driver version
</commit_message>
<xml_diff>
--- a/Bryan spul/assetlist borrelbrouwer v2.xlsx
+++ b/Bryan spul/assetlist borrelbrouwer v2.xlsx
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>